<commit_message>
changed the if from sunday to monday
</commit_message>
<xml_diff>
--- a/Dates.xlsx
+++ b/Dates.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>06-02-2022</t>
+          <t>07-02-2022</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>13-02-2022</t>
+          <t>14-02-2022</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>20-02-2022</t>
+          <t>21-02-2022</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>27-02-2022</t>
+          <t>28-02-2022</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06-03-2022</t>
+          <t>07-03-2022</t>
         </is>
       </c>
     </row>
@@ -544,7 +544,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>13-03-2022</t>
+          <t>14-03-2022</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>20-03-2022</t>
+          <t>21-03-2022</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>27-03-2022</t>
+          <t>28-03-2022</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>03-04-2022</t>
+          <t>04-04-2022</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10-04-2022</t>
+          <t>11-04-2022</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17-04-2022</t>
+          <t>18-04-2022</t>
         </is>
       </c>
     </row>
@@ -664,7 +664,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>24-04-2022</t>
+          <t>25-04-2022</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>01-05-2022</t>
+          <t>02-05-2022</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>08-05-2022</t>
+          <t>09-05-2022</t>
         </is>
       </c>
     </row>
@@ -724,7 +724,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15-05-2022</t>
+          <t>16-05-2022</t>
         </is>
       </c>
     </row>

</xml_diff>